<commit_message>
add 18 april data
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -24,64 +24,509 @@
     <author>nuha</author>
   </authors>
   <commentList>
-    <comment ref="AE27" authorId="0">
+    <comment ref="Y31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>11</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>190
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ28" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y28" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J28" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>160</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="K29" authorId="0">
+      <text>
+        <t>75</t>
+      </text>
+    </comment>
+    <comment ref="G29" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="J25" authorId="0">
+      <text>
+        <t>12</t>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0">
+      <text>
+        <t>47</t>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ3" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="0">
       <text>
         <t>1</t>
       </text>
     </comment>
-    <comment ref="Y27" authorId="0">
+    <comment ref="J3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="AJ4" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <t>32</t>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="AJ5" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <t>40</t>
+      </text>
+    </comment>
+    <comment ref="AJ7" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0">
       <text>
         <t>44</t>
       </text>
     </comment>
-    <comment ref="T27" authorId="0">
+    <comment ref="AB8" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ9" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AB10" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ10" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <t>83</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="AG12" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="J27" authorId="0">
-      <text>
-        <t>29</t>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="0">
+    <comment ref="AJ12" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Z13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ13" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y13" authorId="0">
+      <text>
+        <t>15</t>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0">
+      <text>
+        <t>48</t>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="P14" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <t>25</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0">
+      <text>
+        <t>24
+</t>
+      </text>
+    </comment>
+    <comment ref="Z15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="W15" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <t>41</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <t>14</t>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0">
+      <text>
+        <t>21</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0">
+      <text>
+        <t>62</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AJ17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AA18" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="X18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="O18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="L18" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0">
+      <text>
+        <t>74</t>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AG19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
       <text>
         <t>96</t>
       </text>
     </comment>
-    <comment ref="AB24" authorId="0">
+    <comment ref="C20" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="Z21" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="AJ24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="R24" authorId="0">
-      <text>
-        <t>13</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ20" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y23" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="X23" authorId="0">
-      <text>
-        <t>4</t>
+    <comment ref="Y21" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="0">
+      <text>
+        <t>2</t>
       </text>
     </comment>
     <comment ref="H21" authorId="0">
@@ -90,380 +535,64 @@
 </t>
       </text>
     </comment>
-    <comment ref="M21" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="Y21" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="Z21" authorId="0">
+    <comment ref="X23" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y23" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="H20" authorId="0">
+    <comment ref="AJ20" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <t>13</t>
+      </text>
+    </comment>
+    <comment ref="AJ24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AB24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H27" authorId="0">
       <text>
         <t>96</t>
       </text>
     </comment>
-    <comment ref="X19" authorId="0">
+    <comment ref="J27" authorId="0">
+      <text>
+        <t>29</t>
+      </text>
+    </comment>
+    <comment ref="T27" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="Y19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AG19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0">
-      <text>
-        <t>74</t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="K18" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="O18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="X18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AA18" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="L17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <t>62</t>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0">
-      <text>
-        <t>21</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="0">
-      <text>
-        <t>14</t>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <t>41</t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="W15" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="Y15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Z15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <t>24
-</t>
-      </text>
-    </comment>
-    <comment ref="J14" authorId="0">
-      <text>
-        <t>25</t>
-      </text>
-    </comment>
-    <comment ref="K14" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <t>48</t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="Y13" authorId="0">
-      <text>
-        <t>15</t>
-      </text>
-    </comment>
-    <comment ref="AJ13" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Z13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ12" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AG12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0">
-      <text>
-        <t>83</t>
-      </text>
-    </comment>
-    <comment ref="AJ10" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB10" authorId="0">
+    <comment ref="Y27" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="AE27" authorId="0">
       <text>
         <t>1</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AJ9" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB8" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="Y7" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ7" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0">
-      <text>
-        <t>40</t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ5" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0">
-      <text>
-        <t>32</t>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AJ4" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AB3" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ3" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ6" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H25" authorId="0">
-      <text>
-        <t>47</t>
-      </text>
-    </comment>
-    <comment ref="J25" authorId="0">
-      <text>
-        <t>12</t>
-      </text>
-    </comment>
-    <comment ref="D29" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="K29" authorId="0">
-      <text>
-        <t>75</t>
-      </text>
-    </comment>
-    <comment ref="AA29" authorId="0">
-      <text>
-        <t>0</t>
       </text>
     </comment>
   </commentList>
@@ -560,10 +689,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IS31"/>
+  <dimension ref="A1:IS36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="B33" sqref="B33:AJ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3843,10 +3972,10 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-      <c r="E28">
+      <c r="D28" s="4">
+        <v>-5</v>
+      </c>
+      <c r="E28" s="5">
         <v>0</v>
       </c>
       <c r="F28">
@@ -3855,14 +3984,14 @@
       <c r="G28">
         <v>16</v>
       </c>
-      <c r="H28">
-        <v>160</v>
+      <c r="H28" s="4">
+        <v>179</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28">
-        <v>60</v>
+      <c r="J28" s="4">
+        <v>50</v>
       </c>
       <c r="K28">
         <v>3</v>
@@ -3906,8 +4035,8 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28">
-        <v>0</v>
+      <c r="Y28" s="4">
+        <v>-1</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -3939,8 +4068,8 @@
       <c r="AI28">
         <v>0</v>
       </c>
-      <c r="AJ28">
-        <v>0</v>
+      <c r="AJ28" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:253" ht="13.5">
@@ -4173,8 +4302,8 @@
       <c r="C31">
         <v>15</v>
       </c>
-      <c r="D31">
-        <v>16</v>
+      <c r="D31" s="4">
+        <v>19</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -4182,20 +4311,20 @@
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>196</v>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
+        <v>187</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="J31">
-        <v>11</v>
-      </c>
-      <c r="K31">
-        <v>8</v>
+      <c r="J31" s="4">
+        <v>15</v>
+      </c>
+      <c r="K31" s="4">
+        <v>7</v>
       </c>
       <c r="L31">
         <v>15</v>
@@ -4215,8 +4344,8 @@
       <c r="Q31">
         <v>8</v>
       </c>
-      <c r="R31">
-        <v>6</v>
+      <c r="R31" s="4">
+        <v>7</v>
       </c>
       <c r="S31">
         <v>8</v>
@@ -4233,20 +4362,20 @@
       <c r="W31">
         <v>1</v>
       </c>
-      <c r="X31">
-        <v>2</v>
-      </c>
-      <c r="Y31">
-        <v>29</v>
+      <c r="X31" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y31" s="4">
+        <v>28</v>
       </c>
       <c r="Z31">
         <v>0</v>
       </c>
-      <c r="AA31">
+      <c r="AA31" s="4">
+        <v>6</v>
+      </c>
+      <c r="AB31" s="4">
         <v>5</v>
-      </c>
-      <c r="AB31">
-        <v>4</v>
       </c>
       <c r="AC31">
         <v>0</v>
@@ -4269,10 +4398,122 @@
       <c r="AI31">
         <v>3</v>
       </c>
-      <c r="AJ31">
-        <v>0</v>
+      <c r="AJ31" s="4">
+        <v>-1</v>
       </c>
     </row>
+    <row r="32" spans="1:253" ht="13.5">
+      <c r="A32" s="6">
+        <v>43938</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>154</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>58</v>
+      </c>
+      <c r="K32">
+        <v>5</v>
+      </c>
+      <c r="L32">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>15</v>
+      </c>
+      <c r="Q32">
+        <v>19</v>
+      </c>
+      <c r="R32">
+        <v>19</v>
+      </c>
+      <c r="S32">
+        <v>6</v>
+      </c>
+      <c r="T32">
+        <v>17</v>
+      </c>
+      <c r="U32">
+        <v>7</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>62</v>
+      </c>
+      <c r="Z32">
+        <v>2</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>1</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <v>9</v>
+      </c>
+      <c r="AG32">
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:253" ht="13.5"/>
+    <row r="36" spans="1:253" ht="13.5"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>

</xml_diff>

<commit_message>
update 19 april data
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -26,131 +26,83 @@
   <commentList>
     <comment ref="Y31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>29</t>
-        </r>
+        <t>29</t>
       </text>
     </comment>
     <comment ref="AA31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>5</t>
-        </r>
+        <t>5</t>
       </text>
     </comment>
     <comment ref="AB31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>4</t>
-        </r>
+        <t>4</t>
       </text>
     </comment>
     <comment ref="AJ31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>0</t>
-        </r>
+        <t>0</t>
       </text>
     </comment>
     <comment ref="X31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>2</t>
-        </r>
+        <t>2</t>
       </text>
     </comment>
     <comment ref="R31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>6</t>
-        </r>
+        <t>6</t>
       </text>
     </comment>
     <comment ref="K31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>8</t>
-        </r>
+        <t>8</t>
       </text>
     </comment>
     <comment ref="J31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>11</t>
-        </r>
+        <t>11</t>
       </text>
     </comment>
     <comment ref="H31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>190
+        <t>190
 </t>
-        </r>
       </text>
     </comment>
     <comment ref="G31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>0</t>
-        </r>
+        <t>0</t>
       </text>
     </comment>
     <comment ref="D31" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>16</t>
-        </r>
+        <t>16</t>
       </text>
     </comment>
     <comment ref="AJ28" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>0</t>
-        </r>
+        <t>0</t>
       </text>
     </comment>
     <comment ref="Y28" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>0</t>
-        </r>
+        <t>0</t>
       </text>
     </comment>
     <comment ref="J28" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>60</t>
-        </r>
+        <t>60</t>
       </text>
     </comment>
     <comment ref="H28" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>160</t>
-        </r>
+        <t>160</t>
       </text>
     </comment>
     <comment ref="D28" authorId="0">
       <text>
-        <r>
-          <rPr/>
-          <t>4</t>
-        </r>
+        <t>4</t>
       </text>
     </comment>
     <comment ref="AA29" authorId="0">
@@ -692,7 +644,7 @@
   <dimension ref="A1:IS36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B33" sqref="B33:AJ33"/>
+      <selection activeCell="AK34" sqref="AK34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4512,7 +4464,226 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:253" ht="13.5"/>
+    <row r="33" spans="1:253" ht="13.5">
+      <c r="A33" s="6">
+        <v>43939</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>109</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>9</v>
+      </c>
+      <c r="K33">
+        <v>25</v>
+      </c>
+      <c r="L33">
+        <v>33</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>10</v>
+      </c>
+      <c r="O33">
+        <v>6</v>
+      </c>
+      <c r="P33">
+        <v>18</v>
+      </c>
+      <c r="Q33">
+        <v>3</v>
+      </c>
+      <c r="R33">
+        <v>21</v>
+      </c>
+      <c r="S33">
+        <v>4</v>
+      </c>
+      <c r="T33">
+        <v>30</v>
+      </c>
+      <c r="U33">
+        <v>9</v>
+      </c>
+      <c r="V33">
+        <v>2</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+      <c r="Y33">
+        <v>11</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <v>4</v>
+      </c>
+      <c r="AC33">
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <v>3</v>
+      </c>
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <v>6</v>
+      </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:253" ht="13.5">
+      <c r="A34" s="6">
+        <v>43940</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>108</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>55</v>
+      </c>
+      <c r="K34">
+        <v>20</v>
+      </c>
+      <c r="L34">
+        <v>35</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>5</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
+      </c>
+      <c r="P34">
+        <v>4</v>
+      </c>
+      <c r="Q34">
+        <v>19</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>6</v>
+      </c>
+      <c r="T34">
+        <v>5</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>2</v>
+      </c>
+      <c r="X34">
+        <v>9</v>
+      </c>
+      <c r="Y34">
+        <v>27</v>
+      </c>
+      <c r="Z34">
+        <v>3</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <v>2</v>
+      </c>
+      <c r="AF34">
+        <v>12</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+    </row>
     <row r="36" spans="1:253" ht="13.5"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
update 20 april data
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -24,44 +24,522 @@
     <author>nuha</author>
   </authors>
   <commentList>
-    <comment ref="Y31" authorId="0">
+    <comment ref="AJ34" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>20
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>55</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>108</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE27" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="Y27" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="T27" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="J27" authorId="0">
       <text>
         <t>29</t>
       </text>
     </comment>
-    <comment ref="AA31" authorId="0">
+    <comment ref="H27" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="AB24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <t>13</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ20" authorId="0">
       <text>
         <t>5</t>
       </text>
     </comment>
-    <comment ref="AB31" authorId="0">
+    <comment ref="Y23" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X23" authorId="0">
       <text>
         <t>4</t>
       </text>
     </comment>
-    <comment ref="AJ31" authorId="0">
+    <comment ref="H21" authorId="0">
+      <text>
+        <t>101
+</t>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="Y21" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="Z21" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="X31" authorId="0">
+    <comment ref="C20" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="X19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AG19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0">
+      <text>
+        <t>74</t>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0">
       <text>
         <t>2</t>
       </text>
     </comment>
-    <comment ref="R31" authorId="0">
+    <comment ref="K18" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="L18" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="O18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="X18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="AA18" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AJ18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0">
+      <text>
+        <t>62</t>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0">
+      <text>
+        <t>21</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <t>14</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <t>41</t>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="W15" authorId="0">
       <text>
         <t>6</t>
       </text>
     </comment>
-    <comment ref="K31" authorId="0">
+    <comment ref="Y15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Z15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0">
+      <text>
+        <t>24
+</t>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <t>25</t>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="P14" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0">
+      <text>
+        <t>48</t>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0">
       <text>
         <t>8</t>
       </text>
     </comment>
-    <comment ref="J31" authorId="0">
+    <comment ref="Y13" authorId="0">
+      <text>
+        <t>15</t>
+      </text>
+    </comment>
+    <comment ref="AJ13" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Z13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ12" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AG12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <t>83</t>
+      </text>
+    </comment>
+    <comment ref="AJ10" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="AB10" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
       <text>
         <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AJ9" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="AB8" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ7" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <t>40</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AJ5" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <t>32</t>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="AJ4" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ3" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0">
+      <text>
+        <t>47</t>
+      </text>
+    </comment>
+    <comment ref="J25" authorId="0">
+      <text>
+        <t>12</t>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="G29" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="K29" authorId="0">
+      <text>
+        <t>75</t>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0">
+      <text>
+        <t>160</t>
+      </text>
+    </comment>
+    <comment ref="J28" authorId="0">
+      <text>
+        <t>60</t>
+      </text>
+    </comment>
+    <comment ref="Y28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <t>0</t>
       </text>
     </comment>
     <comment ref="H31" authorId="0">
@@ -70,481 +548,44 @@
 </t>
       </text>
     </comment>
-    <comment ref="G31" authorId="0">
+    <comment ref="J31" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="K31" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="R31" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="X31" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AJ31" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="D31" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="AJ28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0">
-      <text>
-        <t>60</t>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0">
-      <text>
-        <t>160</t>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0">
+    <comment ref="AB31" authorId="0">
       <text>
         <t>4</t>
       </text>
     </comment>
-    <comment ref="AA29" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="K29" authorId="0">
-      <text>
-        <t>75</t>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
+    <comment ref="AA31" authorId="0">
       <text>
         <t>5</t>
       </text>
     </comment>
-    <comment ref="D29" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="J25" authorId="0">
-      <text>
-        <t>12</t>
-      </text>
-    </comment>
-    <comment ref="H25" authorId="0">
-      <text>
-        <t>47</t>
-      </text>
-    </comment>
-    <comment ref="AJ6" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ3" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB3" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="AJ4" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0">
-      <text>
-        <t>32</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AJ5" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0">
-      <text>
-        <t>40</t>
-      </text>
-    </comment>
-    <comment ref="AJ7" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Y7" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="AB8" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ9" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AB10" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ10" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0">
-      <text>
-        <t>83</t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="AG12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ12" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Z13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ13" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Y13" authorId="0">
-      <text>
-        <t>15</t>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <t>48</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="K14" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="J14" authorId="0">
-      <text>
-        <t>25</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <t>24
-</t>
-      </text>
-    </comment>
-    <comment ref="Z15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="W15" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <t>41</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="0">
-      <text>
-        <t>14</t>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0">
-      <text>
-        <t>21</t>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <t>62</t>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AJ17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="L17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AA18" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="X18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="O18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="K18" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0">
-      <text>
-        <t>74</t>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AG19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="X19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H20" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="C20" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="Z21" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y21" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="M21" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H21" authorId="0">
-      <text>
-        <t>101
-</t>
-      </text>
-    </comment>
-    <comment ref="X23" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Y23" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ20" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="R24" authorId="0">
-      <text>
-        <t>13</t>
-      </text>
-    </comment>
-    <comment ref="AJ24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="J27" authorId="0">
+    <comment ref="Y31" authorId="0">
       <text>
         <t>29</t>
-      </text>
-    </comment>
-    <comment ref="T27" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y27" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="AE27" authorId="0">
-      <text>
-        <t>1</t>
       </text>
     </comment>
   </commentList>
@@ -644,7 +685,7 @@
   <dimension ref="A1:IS36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="AK34" sqref="AK34"/>
+      <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4584,8 +4625,8 @@
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34">
-        <v>3</v>
+      <c r="D34" s="4">
+        <v>-9</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -4596,17 +4637,17 @@
       <c r="G34">
         <v>0</v>
       </c>
-      <c r="H34">
-        <v>108</v>
+      <c r="H34" s="4">
+        <v>94</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
-      <c r="J34">
-        <v>55</v>
-      </c>
-      <c r="K34">
-        <v>20</v>
+      <c r="J34" s="4">
+        <v>81</v>
+      </c>
+      <c r="K34" s="4">
+        <v>19</v>
       </c>
       <c r="L34">
         <v>35</v>
@@ -4680,7 +4721,117 @@
       <c r="AI34">
         <v>0</v>
       </c>
-      <c r="AJ34">
+      <c r="AJ34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:253" ht="13.5">
+      <c r="A35" s="6">
+        <v>43941</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>29</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>79</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>25</v>
+      </c>
+      <c r="K35">
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>14</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>5</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>11</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>2</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>2</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <v>4</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <v>0</v>
+      </c>
+      <c r="AJ35">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update data 21 april
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -24,105 +24,461 @@
     <author>nuha</author>
   </authors>
   <commentList>
-    <comment ref="AJ34" authorId="0">
-      <text>
-        <r>
-          <rPr/>
-          <t>0</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K34" authorId="0">
-      <text>
-        <r>
-          <rPr/>
-          <t>20
+    <comment ref="Y31" authorId="0">
+      <text>
+        <t>29</t>
+      </text>
+    </comment>
+    <comment ref="AA31" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="AB31" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AJ31" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X31" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="R31" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="K31" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="J31" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="H31" authorId="0">
+      <text>
+        <t>190
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J34" authorId="0">
-      <text>
-        <r>
-          <rPr/>
-          <t>55</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H34" authorId="0">
-      <text>
-        <r>
-          <rPr/>
-          <t>108</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D34" authorId="0">
-      <text>
-        <r>
-          <rPr/>
-          <t>3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AE27" authorId="0">
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="AJ28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="J28" authorId="0">
+      <text>
+        <t>60</t>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0">
+      <text>
+        <t>160</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="K29" authorId="0">
+      <text>
+        <t>75</t>
+      </text>
+    </comment>
+    <comment ref="G29" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="J25" authorId="0">
+      <text>
+        <t>12</t>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0">
+      <text>
+        <t>47</t>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ3" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="0">
       <text>
         <t>1</t>
       </text>
     </comment>
-    <comment ref="Y27" authorId="0">
+    <comment ref="J3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="AJ4" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <t>32</t>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="AJ5" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <t>40</t>
+      </text>
+    </comment>
+    <comment ref="AJ7" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0">
       <text>
         <t>44</t>
       </text>
     </comment>
-    <comment ref="T27" authorId="0">
+    <comment ref="AB8" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ9" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AB10" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ10" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <t>83</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="AG12" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="J27" authorId="0">
-      <text>
-        <t>29</t>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="0">
+    <comment ref="AJ12" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Z13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ13" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y13" authorId="0">
+      <text>
+        <t>15</t>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0">
+      <text>
+        <t>48</t>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="P14" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <t>25</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0">
+      <text>
+        <t>24
+</t>
+      </text>
+    </comment>
+    <comment ref="Z15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="W15" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <t>41</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <t>14</t>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0">
+      <text>
+        <t>21</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0">
+      <text>
+        <t>62</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AJ17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AA18" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="X18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="O18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="L18" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0">
+      <text>
+        <t>74</t>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AG19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
       <text>
         <t>96</t>
       </text>
     </comment>
-    <comment ref="AB24" authorId="0">
+    <comment ref="C20" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="Z21" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="AJ24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="R24" authorId="0">
-      <text>
-        <t>13</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ20" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y23" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="X23" authorId="0">
-      <text>
-        <t>4</t>
+    <comment ref="Y21" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="0">
+      <text>
+        <t>2</t>
       </text>
     </comment>
     <comment ref="H21" authorId="0">
@@ -131,461 +487,90 @@
 </t>
       </text>
     </comment>
-    <comment ref="M21" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="Y21" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="Z21" authorId="0">
+    <comment ref="X23" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y23" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
+    <comment ref="AJ20" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <t>13</t>
+      </text>
+    </comment>
+    <comment ref="AJ24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AB24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H27" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="J27" authorId="0">
+      <text>
+        <t>29</t>
+      </text>
+    </comment>
+    <comment ref="T27" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y27" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="AE27" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
       <text>
         <t>3</t>
       </text>
     </comment>
-    <comment ref="H20" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="X19" authorId="0">
+    <comment ref="H34" authorId="0">
+      <text>
+        <t>108</t>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0">
+      <text>
+        <t>55</t>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="0">
+      <text>
+        <t>20
+</t>
+      </text>
+    </comment>
+    <comment ref="AJ34" authorId="0">
       <text>
         <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AG19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0">
-      <text>
-        <t>74</t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="K18" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="O18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="X18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AA18" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="L17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <t>62</t>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0">
-      <text>
-        <t>21</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="0">
-      <text>
-        <t>14</t>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <t>41</t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="W15" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="Y15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Z15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <t>24
-</t>
-      </text>
-    </comment>
-    <comment ref="J14" authorId="0">
-      <text>
-        <t>25</t>
-      </text>
-    </comment>
-    <comment ref="K14" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <t>48</t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="Y13" authorId="0">
-      <text>
-        <t>15</t>
-      </text>
-    </comment>
-    <comment ref="AJ13" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Z13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ12" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AG12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0">
-      <text>
-        <t>83</t>
-      </text>
-    </comment>
-    <comment ref="AJ10" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB10" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AJ9" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB8" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="Y7" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ7" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0">
-      <text>
-        <t>40</t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ5" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0">
-      <text>
-        <t>32</t>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AJ4" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AB3" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ3" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ6" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H25" authorId="0">
-      <text>
-        <t>47</t>
-      </text>
-    </comment>
-    <comment ref="J25" authorId="0">
-      <text>
-        <t>12</t>
-      </text>
-    </comment>
-    <comment ref="D29" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="K29" authorId="0">
-      <text>
-        <t>75</t>
-      </text>
-    </comment>
-    <comment ref="AA29" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0">
-      <text>
-        <t>160</t>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0">
-      <text>
-        <t>60</t>
-      </text>
-    </comment>
-    <comment ref="Y28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D31" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="G31" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H31" authorId="0">
-      <text>
-        <t>190
-</t>
-      </text>
-    </comment>
-    <comment ref="J31" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="K31" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="R31" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="X31" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AJ31" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB31" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AA31" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y31" authorId="0">
-      <text>
-        <t>29</t>
       </text>
     </comment>
   </commentList>
@@ -682,10 +667,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IS36"/>
+  <dimension ref="A1:IS40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="Y37" sqref="Y37"/>
+      <selection activeCell="AK36" sqref="AK36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4835,7 +4820,117 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:253" ht="13.5"/>
+    <row r="36" spans="1:253" ht="13.5">
+      <c r="A36" s="6">
+        <v>43942</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>163</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>9</v>
+      </c>
+      <c r="K36">
+        <v>98</v>
+      </c>
+      <c r="L36">
+        <v>13</v>
+      </c>
+      <c r="M36">
+        <v>6</v>
+      </c>
+      <c r="N36">
+        <v>5</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36">
+        <v>2</v>
+      </c>
+      <c r="S36">
+        <v>21</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>2</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>4</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>1</v>
+      </c>
+      <c r="AB36">
+        <v>1</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>11</v>
+      </c>
+      <c r="AG36">
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <v>3</v>
+      </c>
+      <c r="AJ36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:253" ht="13.5"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>

</xml_diff>

<commit_message>
update data 22 april
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -24,44 +24,507 @@
     <author>nuha</author>
   </authors>
   <commentList>
-    <comment ref="Y31" authorId="0">
+    <comment ref="AJ34" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="0">
+      <text>
+        <t>20
+</t>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0">
+      <text>
+        <t>55</t>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="0">
+      <text>
+        <t>108</t>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="AE27" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="Y27" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="T27" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="J27" authorId="0">
       <text>
         <t>29</t>
       </text>
     </comment>
-    <comment ref="AA31" authorId="0">
+    <comment ref="H27" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="AB24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <t>13</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ20" authorId="0">
       <text>
         <t>5</t>
       </text>
     </comment>
-    <comment ref="AB31" authorId="0">
+    <comment ref="Y23" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X23" authorId="0">
       <text>
         <t>4</t>
       </text>
     </comment>
-    <comment ref="AJ31" authorId="0">
+    <comment ref="H21" authorId="0">
+      <text>
+        <t>101
+</t>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="Y21" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="Z21" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="X31" authorId="0">
+    <comment ref="C20" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="X19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AG19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0">
+      <text>
+        <t>74</t>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0">
       <text>
         <t>2</t>
       </text>
     </comment>
-    <comment ref="R31" authorId="0">
+    <comment ref="K18" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="L18" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="O18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="X18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="AA18" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AJ18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0">
+      <text>
+        <t>62</t>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0">
+      <text>
+        <t>21</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <t>14</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <t>41</t>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="W15" authorId="0">
       <text>
         <t>6</t>
       </text>
     </comment>
-    <comment ref="K31" authorId="0">
+    <comment ref="Y15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Z15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0">
+      <text>
+        <t>24
+</t>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <t>25</t>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="P14" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0">
+      <text>
+        <t>48</t>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0">
       <text>
         <t>8</t>
       </text>
     </comment>
-    <comment ref="J31" authorId="0">
+    <comment ref="Y13" authorId="0">
+      <text>
+        <t>15</t>
+      </text>
+    </comment>
+    <comment ref="AJ13" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Z13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ12" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AG12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <t>83</t>
+      </text>
+    </comment>
+    <comment ref="AJ10" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="AB10" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
       <text>
         <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AJ9" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="AB8" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ7" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <t>40</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AJ5" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <t>32</t>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="AJ4" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ3" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0">
+      <text>
+        <t>47</t>
+      </text>
+    </comment>
+    <comment ref="J25" authorId="0">
+      <text>
+        <t>12</t>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="G29" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="K29" authorId="0">
+      <text>
+        <t>75</t>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0">
+      <text>
+        <t>160</t>
+      </text>
+    </comment>
+    <comment ref="J28" authorId="0">
+      <text>
+        <t>60</t>
+      </text>
+    </comment>
+    <comment ref="Y28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <t>0</t>
       </text>
     </comment>
     <comment ref="H31" authorId="0">
@@ -70,507 +533,44 @@
 </t>
       </text>
     </comment>
-    <comment ref="G31" authorId="0">
+    <comment ref="J31" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="K31" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="R31" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="X31" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AJ31" authorId="0">
       <text>
         <t>0</t>
       </text>
     </comment>
-    <comment ref="D31" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="AJ28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0">
-      <text>
-        <t>60</t>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0">
-      <text>
-        <t>160</t>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0">
+    <comment ref="AB31" authorId="0">
       <text>
         <t>4</t>
       </text>
     </comment>
-    <comment ref="AA29" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="K29" authorId="0">
-      <text>
-        <t>75</t>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
+    <comment ref="AA31" authorId="0">
       <text>
         <t>5</t>
       </text>
     </comment>
-    <comment ref="D29" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="J25" authorId="0">
-      <text>
-        <t>12</t>
-      </text>
-    </comment>
-    <comment ref="H25" authorId="0">
-      <text>
-        <t>47</t>
-      </text>
-    </comment>
-    <comment ref="AJ6" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ3" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB3" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="AJ4" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0">
-      <text>
-        <t>32</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AJ5" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0">
-      <text>
-        <t>40</t>
-      </text>
-    </comment>
-    <comment ref="AJ7" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Y7" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="AB8" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ9" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AB10" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ10" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0">
-      <text>
-        <t>83</t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="AG12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ12" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Z13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ13" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Y13" authorId="0">
-      <text>
-        <t>15</t>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <t>48</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="K14" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="J14" authorId="0">
-      <text>
-        <t>25</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <t>24
-</t>
-      </text>
-    </comment>
-    <comment ref="Z15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="W15" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <t>41</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="0">
-      <text>
-        <t>14</t>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0">
-      <text>
-        <t>21</t>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <t>62</t>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AJ17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="L17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AA18" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="X18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="O18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="K18" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0">
-      <text>
-        <t>74</t>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AG19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="X19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H20" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="C20" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="Z21" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y21" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="M21" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H21" authorId="0">
-      <text>
-        <t>101
-</t>
-      </text>
-    </comment>
-    <comment ref="X23" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Y23" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ20" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="R24" authorId="0">
-      <text>
-        <t>13</t>
-      </text>
-    </comment>
-    <comment ref="AJ24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="J27" authorId="0">
+    <comment ref="Y31" authorId="0">
       <text>
         <t>29</t>
-      </text>
-    </comment>
-    <comment ref="T27" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y27" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="AE27" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="D34" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="H34" authorId="0">
-      <text>
-        <t>108</t>
-      </text>
-    </comment>
-    <comment ref="J34" authorId="0">
-      <text>
-        <t>55</t>
-      </text>
-    </comment>
-    <comment ref="K34" authorId="0">
-      <text>
-        <t>20
-</t>
-      </text>
-    </comment>
-    <comment ref="AJ34" authorId="0">
-      <text>
-        <t>0</t>
       </text>
     </comment>
   </commentList>
@@ -670,7 +670,7 @@
   <dimension ref="A1:IS40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="AK36" sqref="AK36"/>
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4930,6 +4930,116 @@
         <v>0</v>
       </c>
     </row>
+    <row r="37" spans="1:253" ht="13.5">
+      <c r="A37" s="6">
+        <v>43943</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>119</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+      <c r="K37">
+        <v>30</v>
+      </c>
+      <c r="L37">
+        <v>35</v>
+      </c>
+      <c r="M37">
+        <v>4</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>15</v>
+      </c>
+      <c r="P37">
+        <v>9</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>15</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>5</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>9</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>13</v>
+      </c>
+      <c r="Z37">
+        <v>2</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <v>8</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <v>1</v>
+      </c>
+      <c r="AF37">
+        <v>5</v>
+      </c>
+      <c r="AG37">
+        <v>1</v>
+      </c>
+      <c r="AH37">
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+    </row>
     <row r="40" spans="1:253" ht="13.5"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
update sampai 26 april
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -24,9 +24,574 @@
     <author>nuha</author>
   </authors>
   <commentList>
-    <comment ref="AJ34" authorId="0">
+    <comment ref="J38" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>22</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H38" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>133</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ37" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="0">
+      <text>
+        <r>
+          <rPr/>
+          <t>119</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y31" authorId="0">
+      <text>
+        <t>29</t>
+      </text>
+    </comment>
+    <comment ref="AA31" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="AB31" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AJ31" authorId="0">
       <text>
         <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X31" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="R31" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="K31" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="J31" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="H31" authorId="0">
+      <text>
+        <t>190
+</t>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="AJ28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y28" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="J28" authorId="0">
+      <text>
+        <t>60</t>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0">
+      <text>
+        <t>160</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="K29" authorId="0">
+      <text>
+        <t>75</t>
+      </text>
+    </comment>
+    <comment ref="G29" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="J25" authorId="0">
+      <text>
+        <t>12</t>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0">
+      <text>
+        <t>47</t>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ3" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="AJ4" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <t>32</t>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="AJ5" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <t>40</t>
+      </text>
+    </comment>
+    <comment ref="AJ7" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="AB8" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ9" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AB10" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="AJ10" authorId="0">
+      <text>
+        <t>7</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <t>83</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="AG12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ12" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Z13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ13" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y13" authorId="0">
+      <text>
+        <t>15</t>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0">
+      <text>
+        <t>8</t>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0">
+      <text>
+        <t>48</t>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="P14" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0">
+      <text>
+        <t>17</t>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <t>25</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0">
+      <text>
+        <t>24
+</t>
+      </text>
+    </comment>
+    <comment ref="Z15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y15" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="W15" authorId="0">
+      <text>
+        <t>6</t>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
+      <text>
+        <t>16</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <t>41</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <t>14</t>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0">
+      <text>
+        <t>21</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0">
+      <text>
+        <t>62</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <t>11</t>
+      </text>
+    </comment>
+    <comment ref="AJ17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="AA18" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="X18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="O18" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="L18" authorId="0">
+      <text>
+        <t>52</t>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="0">
+      <text>
+        <t>10</t>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0">
+      <text>
+        <t>74</t>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AG19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="X19" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="Z21" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y21" authorId="0">
+      <text>
+        <t>30</t>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="0">
+      <text>
+        <t>2</t>
+      </text>
+    </comment>
+    <comment ref="H21" authorId="0">
+      <text>
+        <t>101
+</t>
+      </text>
+    </comment>
+    <comment ref="X23" authorId="0">
+      <text>
+        <t>4</t>
+      </text>
+    </comment>
+    <comment ref="Y23" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AJ20" authorId="0">
+      <text>
+        <t>5</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <t>13</t>
+      </text>
+    </comment>
+    <comment ref="AJ24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="AB24" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="H27" authorId="0">
+      <text>
+        <t>96</t>
+      </text>
+    </comment>
+    <comment ref="J27" authorId="0">
+      <text>
+        <t>29</t>
+      </text>
+    </comment>
+    <comment ref="T27" authorId="0">
+      <text>
+        <t>0</t>
+      </text>
+    </comment>
+    <comment ref="Y27" authorId="0">
+      <text>
+        <t>44</t>
+      </text>
+    </comment>
+    <comment ref="AE27" authorId="0">
+      <text>
+        <t>1</t>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <t>3</t>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="0">
+      <text>
+        <t>108</t>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0">
+      <text>
+        <t>55</t>
       </text>
     </comment>
     <comment ref="K34" authorId="0">
@@ -35,542 +600,9 @@
 </t>
       </text>
     </comment>
-    <comment ref="J34" authorId="0">
-      <text>
-        <t>55</t>
-      </text>
-    </comment>
-    <comment ref="H34" authorId="0">
-      <text>
-        <t>108</t>
-      </text>
-    </comment>
-    <comment ref="D34" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AE27" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="Y27" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="T27" authorId="0">
+    <comment ref="AJ34" authorId="0">
       <text>
         <t>0</t>
-      </text>
-    </comment>
-    <comment ref="J27" authorId="0">
-      <text>
-        <t>29</t>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="AB24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="R24" authorId="0">
-      <text>
-        <t>13</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ20" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y23" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="X23" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H21" authorId="0">
-      <text>
-        <t>101
-</t>
-      </text>
-    </comment>
-    <comment ref="M21" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="Y21" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="Z21" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="C20" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="H20" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="X19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AG19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0">
-      <text>
-        <t>74</t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="K18" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="O18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="X18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AA18" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="L17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <t>62</t>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0">
-      <text>
-        <t>21</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="0">
-      <text>
-        <t>14</t>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <t>41</t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="W15" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="Y15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Z15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <t>24
-</t>
-      </text>
-    </comment>
-    <comment ref="J14" authorId="0">
-      <text>
-        <t>25</t>
-      </text>
-    </comment>
-    <comment ref="K14" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <t>48</t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="Y13" authorId="0">
-      <text>
-        <t>15</t>
-      </text>
-    </comment>
-    <comment ref="AJ13" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Z13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ12" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AG12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0">
-      <text>
-        <t>83</t>
-      </text>
-    </comment>
-    <comment ref="AJ10" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB10" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AJ9" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB8" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="Y7" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ7" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0">
-      <text>
-        <t>40</t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ5" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0">
-      <text>
-        <t>32</t>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AJ4" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AB3" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ3" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ6" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H25" authorId="0">
-      <text>
-        <t>47</t>
-      </text>
-    </comment>
-    <comment ref="J25" authorId="0">
-      <text>
-        <t>12</t>
-      </text>
-    </comment>
-    <comment ref="D29" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="K29" authorId="0">
-      <text>
-        <t>75</t>
-      </text>
-    </comment>
-    <comment ref="AA29" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0">
-      <text>
-        <t>160</t>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0">
-      <text>
-        <t>60</t>
-      </text>
-    </comment>
-    <comment ref="Y28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D31" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="G31" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H31" authorId="0">
-      <text>
-        <t>190
-</t>
-      </text>
-    </comment>
-    <comment ref="J31" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="K31" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="R31" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="X31" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AJ31" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB31" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AA31" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y31" authorId="0">
-      <text>
-        <t>29</t>
       </text>
     </comment>
   </commentList>
@@ -667,10 +699,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IS40"/>
+  <dimension ref="A1:IS41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="AK22" sqref="AK22"/>
+    <sheetView topLeftCell="A21" workbookViewId="0" tabSelected="1">
+      <selection activeCell="AK41" sqref="AK41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4952,8 +4984,8 @@
       <c r="G37">
         <v>3</v>
       </c>
-      <c r="H37">
-        <v>119</v>
+      <c r="H37" s="4">
+        <v>120</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -5036,11 +5068,450 @@
       <c r="AI37">
         <v>0</v>
       </c>
-      <c r="AJ37">
-        <v>0</v>
+      <c r="AJ37" s="4">
+        <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:253" ht="13.5"/>
+    <row r="38" spans="1:253" ht="13.5">
+      <c r="A38" s="6">
+        <v>43944</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="4">
+        <v>130</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" s="4">
+        <v>25</v>
+      </c>
+      <c r="K38">
+        <v>59</v>
+      </c>
+      <c r="L38">
+        <v>26</v>
+      </c>
+      <c r="M38">
+        <v>19</v>
+      </c>
+      <c r="N38">
+        <v>5</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>7</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>2</v>
+      </c>
+      <c r="S38">
+        <v>7</v>
+      </c>
+      <c r="T38">
+        <v>4</v>
+      </c>
+      <c r="U38">
+        <v>5</v>
+      </c>
+      <c r="V38">
+        <v>11</v>
+      </c>
+      <c r="W38">
+        <v>2</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>10</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>11</v>
+      </c>
+      <c r="AB38">
+        <v>1</v>
+      </c>
+      <c r="AC38">
+        <v>2</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>5</v>
+      </c>
+      <c r="AF38">
+        <v>7</v>
+      </c>
+      <c r="AG38">
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:253" ht="13.5">
+      <c r="A39" s="6">
+        <v>43945</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>22</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>85</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="J39">
+        <v>75</v>
+      </c>
+      <c r="K39">
+        <v>37</v>
+      </c>
+      <c r="L39">
+        <v>26</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>11</v>
+      </c>
+      <c r="O39">
+        <v>11</v>
+      </c>
+      <c r="P39">
+        <v>18</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>38</v>
+      </c>
+      <c r="T39">
+        <v>13</v>
+      </c>
+      <c r="U39">
+        <v>10</v>
+      </c>
+      <c r="V39">
+        <v>5</v>
+      </c>
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <v>4</v>
+      </c>
+      <c r="Y39">
+        <v>23</v>
+      </c>
+      <c r="Z39">
+        <v>3</v>
+      </c>
+      <c r="AA39">
+        <v>0</v>
+      </c>
+      <c r="AB39">
+        <v>0</v>
+      </c>
+      <c r="AC39">
+        <v>0</v>
+      </c>
+      <c r="AD39">
+        <v>0</v>
+      </c>
+      <c r="AE39">
+        <v>2</v>
+      </c>
+      <c r="AF39">
+        <v>6</v>
+      </c>
+      <c r="AG39">
+        <v>25</v>
+      </c>
+      <c r="AH39">
+        <v>0</v>
+      </c>
+      <c r="AI39">
+        <v>5</v>
+      </c>
+      <c r="AJ39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:253" ht="13.5">
+      <c r="A40" s="6">
+        <v>43946</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>22</v>
+      </c>
+      <c r="H40">
+        <v>85</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>45</v>
+      </c>
+      <c r="K40">
+        <v>46</v>
+      </c>
+      <c r="L40">
+        <v>80</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>12</v>
+      </c>
+      <c r="O40">
+        <v>6</v>
+      </c>
+      <c r="P40">
+        <v>14</v>
+      </c>
+      <c r="Q40">
+        <v>6</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>27</v>
+      </c>
+      <c r="T40">
+        <v>13</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>9</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>12</v>
+      </c>
+      <c r="Z40">
+        <v>4</v>
+      </c>
+      <c r="AA40">
+        <v>0</v>
+      </c>
+      <c r="AB40">
+        <v>22</v>
+      </c>
+      <c r="AC40">
+        <v>0</v>
+      </c>
+      <c r="AD40">
+        <v>5</v>
+      </c>
+      <c r="AE40">
+        <v>1</v>
+      </c>
+      <c r="AF40">
+        <v>0</v>
+      </c>
+      <c r="AG40">
+        <v>2</v>
+      </c>
+      <c r="AH40">
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <v>2</v>
+      </c>
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:253" ht="13.5">
+      <c r="A41" s="6">
+        <v>43947</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>114</v>
+      </c>
+      <c r="I41">
+        <v>11</v>
+      </c>
+      <c r="J41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>28</v>
+      </c>
+      <c r="L41">
+        <v>15</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>8</v>
+      </c>
+      <c r="O41">
+        <v>4</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>6</v>
+      </c>
+      <c r="R41">
+        <v>2</v>
+      </c>
+      <c r="S41">
+        <v>15</v>
+      </c>
+      <c r="T41">
+        <v>10</v>
+      </c>
+      <c r="U41">
+        <v>5</v>
+      </c>
+      <c r="V41">
+        <v>4</v>
+      </c>
+      <c r="W41">
+        <v>6</v>
+      </c>
+      <c r="X41">
+        <v>4</v>
+      </c>
+      <c r="Y41">
+        <v>8</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41">
+        <v>4</v>
+      </c>
+      <c r="AB41">
+        <v>1</v>
+      </c>
+      <c r="AC41">
+        <v>12</v>
+      </c>
+      <c r="AD41">
+        <v>0</v>
+      </c>
+      <c r="AE41">
+        <v>0</v>
+      </c>
+      <c r="AF41">
+        <v>5</v>
+      </c>
+      <c r="AG41">
+        <v>0</v>
+      </c>
+      <c r="AH41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <v>1</v>
+      </c>
+      <c r="AJ41">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>

</xml_diff>

<commit_message>
add recover and dead data and update to 15 may data
</commit_message>
<xml_diff>
--- a/daily_increment_positif.xlsx
+++ b/daily_increment_positif.xlsx
@@ -1,697 +1,321 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="19200" windowHeight="8260"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="provinsi copy.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="provinsi copy.csv" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"provinsi copy.csv"</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>nuha</author>
   </authors>
   <commentList>
-    <comment ref="AJ52" authorId="0">
+    <comment ref="H36" authorId="0">
       <text>
         <r>
-          <rPr/>
-          <t>0</t>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>nuha:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+163</t>
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0">
+    <comment ref="D36" authorId="0">
       <text>
         <r>
-          <rPr/>
-          <t>13</t>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>nuha:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+0</t>
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="0">
+    <comment ref="X58" authorId="0">
       <text>
-        <t>39</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>nuha:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+91</t>
+        </r>
       </text>
     </comment>
-    <comment ref="AI41" authorId="0">
+    <comment ref="Z58" authorId="0">
       <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="H41" authorId="0">
-      <text>
-        <t>114</t>
-      </text>
-    </comment>
-    <comment ref="AJ34" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="K34" authorId="0">
-      <text>
-        <t>20
-</t>
-      </text>
-    </comment>
-    <comment ref="J34" authorId="0">
-      <text>
-        <t>55</t>
-      </text>
-    </comment>
-    <comment ref="H34" authorId="0">
-      <text>
-        <t>108</t>
-      </text>
-    </comment>
-    <comment ref="D34" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AE27" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="Y27" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="T27" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="J27" authorId="0">
-      <text>
-        <t>29</t>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="AB24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="R24" authorId="0">
-      <text>
-        <t>13</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ20" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y23" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="X23" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H21" authorId="0">
-      <text>
-        <t>101
-</t>
-      </text>
-    </comment>
-    <comment ref="M21" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="Y21" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="Z21" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="C20" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="H20" authorId="0">
-      <text>
-        <t>96</t>
-      </text>
-    </comment>
-    <comment ref="X19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AG19" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0">
-      <text>
-        <t>74</t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="K18" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="O18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="X18" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="AA18" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ18" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="L17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ17" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <t>62</t>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0">
-      <text>
-        <t>21</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="0">
-      <text>
-        <t>14</t>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <t>41</t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="W15" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="Y15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Z15" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <t>24
-</t>
-      </text>
-    </comment>
-    <comment ref="J14" authorId="0">
-      <text>
-        <t>25</t>
-      </text>
-    </comment>
-    <comment ref="K14" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <t>48</t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="0">
-      <text>
-        <t>30</t>
-      </text>
-    </comment>
-    <comment ref="K13" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="Y13" authorId="0">
-      <text>
-        <t>15</t>
-      </text>
-    </comment>
-    <comment ref="AJ13" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="Z13" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ12" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AG12" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0">
-      <text>
-        <t>17</t>
-      </text>
-    </comment>
-    <comment ref="H11" authorId="0">
-      <text>
-        <t>83</t>
-      </text>
-    </comment>
-    <comment ref="AJ10" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB10" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="AJ9" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AB8" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0">
-      <text>
-        <t>44</t>
-      </text>
-    </comment>
-    <comment ref="Y7" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ7" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0">
-      <text>
-        <t>40</t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AJ5" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <t>3</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0">
-      <text>
-        <t>32</t>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <t>7</t>
-      </text>
-    </comment>
-    <comment ref="AJ4" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <t>52</t>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AB3" authorId="0">
-      <text>
-        <t>1</t>
-      </text>
-    </comment>
-    <comment ref="AJ3" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ6" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H25" authorId="0">
-      <text>
-        <t>47</t>
-      </text>
-    </comment>
-    <comment ref="J25" authorId="0">
-      <text>
-        <t>12</t>
-      </text>
-    </comment>
-    <comment ref="D29" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="K29" authorId="0">
-      <text>
-        <t>75</t>
-      </text>
-    </comment>
-    <comment ref="AA29" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0">
-      <text>
-        <t>160</t>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0">
-      <text>
-        <t>60</t>
-      </text>
-    </comment>
-    <comment ref="Y28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AJ28" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="D31" authorId="0">
-      <text>
-        <t>16</t>
-      </text>
-    </comment>
-    <comment ref="G31" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H31" authorId="0">
-      <text>
-        <t>190
-</t>
-      </text>
-    </comment>
-    <comment ref="J31" authorId="0">
-      <text>
-        <t>11</t>
-      </text>
-    </comment>
-    <comment ref="K31" authorId="0">
-      <text>
-        <t>8</t>
-      </text>
-    </comment>
-    <comment ref="R31" authorId="0">
-      <text>
-        <t>6</t>
-      </text>
-    </comment>
-    <comment ref="X31" authorId="0">
-      <text>
-        <t>2</t>
-      </text>
-    </comment>
-    <comment ref="AJ31" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="AB31" authorId="0">
-      <text>
-        <t>4</t>
-      </text>
-    </comment>
-    <comment ref="AA31" authorId="0">
-      <text>
-        <t>5</t>
-      </text>
-    </comment>
-    <comment ref="Y31" authorId="0">
-      <text>
-        <t>29</t>
-      </text>
-    </comment>
-    <comment ref="H37" authorId="0">
-      <text>
-        <t>119</t>
-      </text>
-    </comment>
-    <comment ref="AJ37" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H38" authorId="0">
-      <text>
-        <t>133</t>
-      </text>
-    </comment>
-    <comment ref="J38" authorId="0">
-      <text>
-        <t>22</t>
-      </text>
-    </comment>
-    <comment ref="H44" authorId="0">
-      <text>
-        <t>90</t>
-      </text>
-    </comment>
-    <comment ref="AJ44" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="K46" authorId="0">
-      <text>
-        <t>22</t>
-      </text>
-    </comment>
-    <comment ref="AJ46" authorId="0">
-      <text>
-        <t>0</t>
-      </text>
-    </comment>
-    <comment ref="H47" authorId="0">
-      <text>
-        <t>80</t>
-      </text>
-    </comment>
-    <comment ref="J47" authorId="0">
-      <text>
-        <t>31</t>
-      </text>
-    </comment>
-    <comment ref="H48" authorId="0">
-      <text>
-        <t>67</t>
-      </text>
-    </comment>
-    <comment ref="J48" authorId="0">
-      <text>
-        <t>10</t>
-      </text>
-    </comment>
-    <comment ref="AJ48" authorId="0">
-      <text>
-        <t>0</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>nuha:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+6</t>
+        </r>
       </text>
     </comment>
   </commentList>
 </comments>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <r>
+      <t>tanggal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>aceh</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>bali</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>banten</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bangka belitung</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>bengkulu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>yogyakarta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>jakarta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>jambi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jawa barat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jawa tengah</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jawa timur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kalimantan barat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kalimantan timur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kalimantan tengah</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kalimantan selatan</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kalimantan utara</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kepulauan riau</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nusa tenggara barat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sumatera selatan</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sumatera barat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sulawesi utara</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sumatera utara</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sulawesi tenggara</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sulawesi selatan</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sulawesi tengah</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>lampung</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>riau</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">maluku utara</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>maluku</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">papua barat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>papua</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sulawesi barat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nusa tenggara timur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>gorontalo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>proses</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="100"/>
-    <numFmt formatCode="yyyy-mmm-dd" numFmtId="101"/>
+    <numFmt numFmtId="160" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="161" formatCode="yyyy-mmm-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <name val="Sans"/>
       <b val="0"/>
       <i val="0"/>
+      <strike val="0"/>
+      <color indexed="64"/>
+      <sz val="10"/>
       <u val="none"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
       <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,265 +324,598 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor indexed="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+  <cellStyleXfs count="2">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="10">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
+  <a:themeElements>
+    <a:clrScheme name="">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="">
+      <a:majorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill/>
+        <a:solidFill/>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+        </a:ln>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill/>
+        <a:solidFill/>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IS65"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0" tabSelected="1">
-      <selection activeCell="AK58" sqref="AK58"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="AK58" activeCellId="0" sqref="AK58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="12.42782451923077" bestFit="1" customWidth="1"/>
-    <col min="2" max="36" style="0" width="6.571033653846155" customWidth="1"/>
-    <col min="37" max="253" style="0" width="6.999579326923078" bestFit="1" customWidth="1"/>
-    <col min="254" max="16384" style="0" width="9.142307692307693"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="0" width="12.42782451923077"/>
+    <col customWidth="1" min="2" max="36" style="0" width="6.5710336538461549"/>
+    <col bestFit="1" customWidth="1" min="37" max="253" style="0" width="6.9995793269230777"/>
+    <col min="254" max="16384" style="0" width="9.1423076923076927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:253" customHeight="1" ht="47.25">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>tanggal</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>aceh</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>bali</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>banten</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>bangka belitung</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>bengkulu</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>yogyakarta</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>jakarta</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>jambi</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>jawa barat</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>jawa tengah</t>
-        </is>
-      </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>jawa timur</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>kalimantan barat</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>kalimantan timur</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="inlineStr">
-        <is>
-          <t>kalimantan tengah</t>
-        </is>
-      </c>
-      <c r="P1" s="2" t="inlineStr">
-        <is>
-          <t>kalimantan selatan</t>
-        </is>
-      </c>
-      <c r="Q1" s="2" t="inlineStr">
-        <is>
-          <t>kalimantan utara</t>
-        </is>
-      </c>
-      <c r="R1" s="2" t="inlineStr">
-        <is>
-          <t>kepulauan riau</t>
-        </is>
-      </c>
-      <c r="S1" s="2" t="inlineStr">
-        <is>
-          <t>nusa tenggara barat</t>
-        </is>
-      </c>
-      <c r="T1" s="2" t="inlineStr">
-        <is>
-          <t>sumatera selatan</t>
-        </is>
-      </c>
-      <c r="U1" s="2" t="inlineStr">
-        <is>
-          <t>sumatera barat</t>
-        </is>
-      </c>
-      <c r="V1" s="2" t="inlineStr">
-        <is>
-          <t>sulawesi utara</t>
-        </is>
-      </c>
-      <c r="W1" s="2" t="inlineStr">
-        <is>
-          <t>sumatera utara</t>
-        </is>
-      </c>
-      <c r="X1" s="2" t="inlineStr">
-        <is>
-          <t>sulawesi tenggara</t>
-        </is>
-      </c>
-      <c r="Y1" s="2" t="inlineStr">
-        <is>
-          <t>sulawesi selatan</t>
-        </is>
-      </c>
-      <c r="Z1" s="2" t="inlineStr">
-        <is>
-          <t>sulawesi tengah</t>
-        </is>
-      </c>
-      <c r="AA1" s="2" t="inlineStr">
-        <is>
-          <t>lampung</t>
-        </is>
-      </c>
-      <c r="AB1" s="2" t="inlineStr">
-        <is>
-          <t>riau</t>
-        </is>
-      </c>
-      <c r="AC1" s="2" t="inlineStr">
-        <is>
-          <t>maluku utara</t>
-        </is>
-      </c>
-      <c r="AD1" s="2" t="inlineStr">
-        <is>
-          <t>maluku</t>
-        </is>
-      </c>
-      <c r="AE1" s="2" t="inlineStr">
-        <is>
-          <t>papua barat</t>
-        </is>
-      </c>
-      <c r="AF1" s="2" t="inlineStr">
-        <is>
-          <t>papua</t>
-        </is>
-      </c>
-      <c r="AG1" s="2" t="inlineStr">
-        <is>
-          <t>sulawesi barat</t>
-        </is>
-      </c>
-      <c r="AH1" s="2" t="inlineStr">
-        <is>
-          <t>nusa tenggara timur</t>
-        </is>
-      </c>
-      <c r="AI1" s="2" t="inlineStr">
-        <is>
-          <t>gorontalo</t>
-        </is>
-      </c>
-      <c r="AJ1" s="2" t="inlineStr">
-        <is>
-          <t>proses</t>
-        </is>
-      </c>
-      <c r="AK1" s="2"/>
+    <row r="1" ht="47.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="3"/>
       <c r="AL1" s="2"/>
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
@@ -1176,8 +1133,8 @@
       <c r="IR1" s="2"/>
       <c r="IS1" s="2"/>
     </row>
-    <row r="2" spans="1:253">
-      <c r="A2" s="3">
+    <row r="2">
+      <c r="A2" s="4">
         <v>43908</v>
       </c>
       <c r="B2">
@@ -1285,9 +1242,13 @@
       <c r="AJ2">
         <v>0</v>
       </c>
+      <c r="AK2" s="5">
+        <f>SUM(B2:AJ2)</f>
+        <v>227</v>
+      </c>
     </row>
-    <row r="3" spans="1:253" ht="13.5">
-      <c r="A3" s="3">
+    <row r="3" ht="13.5">
+      <c r="A3" s="4">
         <v>43909</v>
       </c>
       <c r="B3">
@@ -1296,7 +1257,7 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>18</v>
       </c>
       <c r="E3">
@@ -1305,16 +1266,16 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
         <v>25</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="6">
         <v>16</v>
       </c>
       <c r="K3">
@@ -1368,7 +1329,7 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="AB3" s="6">
         <v>0</v>
       </c>
       <c r="AC3">
@@ -1392,21 +1353,25 @@
       <c r="AI3">
         <v>0</v>
       </c>
-      <c r="AJ3" s="4">
+      <c r="AJ3" s="6">
         <v>7</v>
       </c>
+      <c r="AK3" s="5">
+        <f>SUM(B3:AJ3)</f>
+        <v>82</v>
+      </c>
     </row>
-    <row r="4" spans="1:253" ht="13.5">
-      <c r="A4" s="3">
+    <row r="4" ht="13.5">
+      <c r="A4" s="4">
         <v>43910</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
         <v>4</v>
       </c>
       <c r="E4">
@@ -1418,7 +1383,7 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6">
         <v>40</v>
       </c>
       <c r="I4">
@@ -1436,7 +1401,7 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="6">
         <v>6</v>
       </c>
       <c r="O4">
@@ -1469,7 +1434,7 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y4" s="6">
         <v>-2</v>
       </c>
       <c r="Z4">
@@ -1502,12 +1467,16 @@
       <c r="AI4">
         <v>0</v>
       </c>
-      <c r="AJ4" s="4">
-        <v>0</v>
+      <c r="AJ4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="5">
+        <f>SUM(B4:AJ4)</f>
+        <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:253" ht="13.5">
-      <c r="A5" s="3">
+    <row r="5" ht="13.5">
+      <c r="A5" s="4">
         <v>43911</v>
       </c>
       <c r="B5">
@@ -1516,7 +1485,7 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>8</v>
       </c>
       <c r="E5">
@@ -1612,12 +1581,16 @@
       <c r="AI5">
         <v>0</v>
       </c>
-      <c r="AJ5" s="4">
+      <c r="AJ5" s="6">
         <v>-1</v>
       </c>
+      <c r="AK5" s="5">
+        <f>SUM(B5:AJ5)</f>
+        <v>81</v>
+      </c>
     </row>
-    <row r="6" spans="1:253" ht="13.5">
-      <c r="A6" s="3">
+    <row r="6" ht="13.5">
+      <c r="A6" s="4">
         <v>43912</v>
       </c>
       <c r="B6">
@@ -1638,7 +1611,7 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="6">
         <v>42</v>
       </c>
       <c r="I6">
@@ -1722,12 +1695,16 @@
       <c r="AI6">
         <v>0</v>
       </c>
-      <c r="AJ6" s="4">
+      <c r="AJ6" s="6">
         <v>-2</v>
       </c>
+      <c r="AK6" s="5">
+        <f>SUM(B6:AJ6)</f>
+        <v>64</v>
+      </c>
     </row>
-    <row r="7" spans="1:253" ht="13.5">
-      <c r="A7" s="3">
+    <row r="7" ht="13.5">
+      <c r="A7" s="4">
         <v>43913</v>
       </c>
       <c r="B7">
@@ -1748,7 +1725,7 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="6">
         <v>45</v>
       </c>
       <c r="I7">
@@ -1799,7 +1776,7 @@
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="6">
         <v>2</v>
       </c>
       <c r="Z7">
@@ -1832,12 +1809,16 @@
       <c r="AI7">
         <v>0</v>
       </c>
-      <c r="AJ7" s="4">
-        <v>1</v>
+      <c r="AJ7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="5">
+        <f>SUM(B7:AJ7)</f>
+        <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:253" ht="13.5">
-      <c r="A8" s="3">
+    <row r="8" ht="13.5">
+      <c r="A8" s="4">
         <v>43914</v>
       </c>
       <c r="B8">
@@ -1918,7 +1899,7 @@
       <c r="AA8">
         <v>0</v>
       </c>
-      <c r="AB8" s="4">
+      <c r="AB8" s="6">
         <v>0</v>
       </c>
       <c r="AC8">
@@ -1945,9 +1926,13 @@
       <c r="AJ8">
         <v>0</v>
       </c>
+      <c r="AK8" s="5">
+        <f>SUM(B8:AJ8)</f>
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:253" ht="13.5">
-      <c r="A9" s="3">
+    <row r="9" ht="13.5">
+      <c r="A9" s="4">
         <v>43915</v>
       </c>
       <c r="B9">
@@ -1965,7 +1950,7 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="6">
         <v>10</v>
       </c>
       <c r="H9">
@@ -2052,12 +2037,16 @@
       <c r="AI9">
         <v>0</v>
       </c>
-      <c r="AJ9" s="4">
+      <c r="AJ9" s="6">
         <v>8</v>
       </c>
+      <c r="AK9" s="5">
+        <f>SUM(B9:AJ9)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="10" spans="1:253" ht="13.5">
-      <c r="A10" s="3">
+    <row r="10" ht="13.5">
+      <c r="A10" s="4">
         <v>43916</v>
       </c>
       <c r="B10">
@@ -2138,7 +2127,7 @@
       <c r="AA10">
         <v>2</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="AB10" s="6">
         <v>0</v>
       </c>
       <c r="AC10">
@@ -2162,12 +2151,16 @@
       <c r="AI10">
         <v>0</v>
       </c>
-      <c r="AJ10" s="4">
+      <c r="AJ10" s="6">
         <v>8</v>
       </c>
+      <c r="AK10" s="5">
+        <f>SUM(B10:AJ10)</f>
+        <v>103</v>
+      </c>
     </row>
-    <row r="11" spans="1:253" ht="13.5">
-      <c r="A11" s="3">
+    <row r="11" ht="13.5">
+      <c r="A11" s="4">
         <v>43917</v>
       </c>
       <c r="B11">
@@ -2176,7 +2169,7 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="6">
         <v>26</v>
       </c>
       <c r="E11">
@@ -2188,7 +2181,7 @@
       <c r="G11">
         <v>6</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="6">
         <v>74</v>
       </c>
       <c r="I11">
@@ -2275,12 +2268,16 @@
       <c r="AJ11">
         <v>7</v>
       </c>
+      <c r="AK11" s="5">
+        <f>SUM(B11:AJ11)</f>
+        <v>153</v>
+      </c>
     </row>
-    <row r="12" spans="1:253" ht="13.5">
-      <c r="A12" s="3">
+    <row r="12" ht="13.5">
+      <c r="A12" s="4">
         <v>43918</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12">
@@ -2325,7 +2322,7 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="7">
         <v>2</v>
       </c>
       <c r="R12">
@@ -2373,7 +2370,7 @@
       <c r="AF12">
         <v>0</v>
       </c>
-      <c r="AG12" s="4">
+      <c r="AG12" s="6">
         <v>1</v>
       </c>
       <c r="AH12">
@@ -2382,12 +2379,16 @@
       <c r="AI12">
         <v>0</v>
       </c>
-      <c r="AJ12" s="4">
-        <v>1</v>
+      <c r="AJ12" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="5">
+        <f>SUM(B12:AJ12)</f>
+        <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:253" ht="13.5">
-      <c r="A13" s="3">
+    <row r="13" ht="13.5">
+      <c r="A13" s="4">
         <v>43919</v>
       </c>
       <c r="B13">
@@ -2405,19 +2406,19 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="6">
         <v>-5</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="6">
         <v>47</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="6">
         <v>36</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="6">
         <v>9</v>
       </c>
       <c r="L13">
@@ -2459,10 +2460,10 @@
       <c r="X13">
         <v>0</v>
       </c>
-      <c r="Y13" s="4">
+      <c r="Y13" s="6">
         <v>13</v>
       </c>
-      <c r="Z13" s="4">
+      <c r="Z13" s="6">
         <v>1</v>
       </c>
       <c r="AA13">
@@ -2492,12 +2493,16 @@
       <c r="AI13">
         <v>0</v>
       </c>
-      <c r="AJ13" s="4">
+      <c r="AJ13" s="6">
         <v>3</v>
       </c>
+      <c r="AK13" s="5">
+        <f>SUM(B13:AJ13)</f>
+        <v>129</v>
+      </c>
     </row>
-    <row r="14" spans="1:253" ht="13.5">
-      <c r="A14" s="3">
+    <row r="14" ht="13.5">
+      <c r="A14" s="4">
         <v>43920</v>
       </c>
       <c r="B14">
@@ -2518,16 +2523,16 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="6">
         <v>32</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="6">
         <v>27</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="6">
         <v>16</v>
       </c>
       <c r="L14">
@@ -2542,7 +2547,7 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="6">
         <v>5</v>
       </c>
       <c r="Q14">
@@ -2605,9 +2610,13 @@
       <c r="AJ14">
         <v>-5</v>
       </c>
+      <c r="AK14" s="5">
+        <f>SUM(B14:AJ14)</f>
+        <v>129</v>
+      </c>
     </row>
-    <row r="15" spans="1:253" ht="13.5">
-      <c r="A15" s="3">
+    <row r="15" ht="13.5">
+      <c r="A15" s="4">
         <v>43921</v>
       </c>
       <c r="B15">
@@ -2616,7 +2625,7 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="6">
         <v>13</v>
       </c>
       <c r="E15">
@@ -2628,13 +2637,13 @@
       <c r="G15">
         <v>5</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="6">
         <v>40</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="6">
         <v>17</v>
       </c>
       <c r="K15">
@@ -2673,16 +2682,16 @@
       <c r="V15">
         <v>0</v>
       </c>
-      <c r="W15" s="4">
+      <c r="W15" s="6">
         <v>7</v>
       </c>
       <c r="X15">
         <v>0</v>
       </c>
-      <c r="Y15" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="4">
+      <c r="Y15" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="6">
         <v>-1</v>
       </c>
       <c r="AA15">
@@ -2715,9 +2724,13 @@
       <c r="AJ15">
         <v>1</v>
       </c>
+      <c r="AK15" s="5">
+        <f>SUM(B15:AJ15)</f>
+        <v>114</v>
+      </c>
     </row>
-    <row r="16" spans="1:253" ht="13.5">
-      <c r="A16" s="3">
+    <row r="16" ht="13.5">
+      <c r="A16" s="4">
         <v>43922</v>
       </c>
       <c r="B16">
@@ -2726,7 +2739,7 @@
       <c r="C16">
         <v>6</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="6">
         <v>15</v>
       </c>
       <c r="E16">
@@ -2735,16 +2748,16 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="6">
         <v>4</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="6">
         <v>71</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="6">
         <v>9</v>
       </c>
       <c r="K16">
@@ -2825,9 +2838,13 @@
       <c r="AJ16">
         <v>0</v>
       </c>
+      <c r="AK16" s="5">
+        <f>SUM(B16:AJ16)</f>
+        <v>149</v>
+      </c>
     </row>
-    <row r="17" spans="1:253" ht="13.5">
-      <c r="A17" s="3">
+    <row r="17" ht="13.5">
+      <c r="A17" s="4">
         <v>43923</v>
       </c>
       <c r="B17">
@@ -2860,7 +2877,7 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="6">
         <v>-1</v>
       </c>
       <c r="M17">
@@ -2932,12 +2949,16 @@
       <c r="AI17">
         <v>0</v>
       </c>
-      <c r="AJ17" s="4">
-        <v>1</v>
+      <c r="AJ17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="5">
+        <f>SUM(B17:AJ17)</f>
+        <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:253" ht="13.5">
-      <c r="A18" s="3">
+    <row r="18" ht="13.5">
+      <c r="A18" s="4">
         <v>43924</v>
       </c>
       <c r="B18">
@@ -2955,22 +2976,22 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6">
         <v>76</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="J18" s="6">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
         <v>9</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="6">
         <v>49</v>
       </c>
       <c r="M18">
@@ -2979,7 +3000,7 @@
       <c r="N18">
         <v>1</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="6">
         <v>2</v>
       </c>
       <c r="P18">
@@ -3006,7 +3027,7 @@
       <c r="W18">
         <v>0</v>
       </c>
-      <c r="X18" s="4">
+      <c r="X18" s="6">
         <v>2</v>
       </c>
       <c r="Y18">
@@ -3015,7 +3036,7 @@
       <c r="Z18">
         <v>2</v>
       </c>
-      <c r="AA18" s="4">
+      <c r="AA18" s="6">
         <v>3</v>
       </c>
       <c r="AB18">
@@ -3042,12 +3063,16 @@
       <c r="AI18">
         <v>0</v>
       </c>
-      <c r="AJ18" s="4">
+      <c r="AJ18" s="6">
         <v>8</v>
       </c>
+      <c r="AK18" s="5">
+        <f>SUM(B18:AJ18)</f>
+        <v>196</v>
+      </c>
     </row>
-    <row r="19" spans="1:253" ht="13.5">
-      <c r="A19" s="3">
+    <row r="19" ht="13.5">
+      <c r="A19" s="4">
         <v>43925</v>
       </c>
       <c r="B19">
@@ -3116,10 +3141,10 @@
       <c r="W19">
         <v>3</v>
       </c>
-      <c r="X19" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="4">
+      <c r="X19" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="6">
         <v>-2</v>
       </c>
       <c r="Z19">
@@ -3143,7 +3168,7 @@
       <c r="AF19">
         <v>2</v>
       </c>
-      <c r="AG19" s="4">
+      <c r="AG19" s="6">
         <v>1</v>
       </c>
       <c r="AH19">
@@ -3155,15 +3180,19 @@
       <c r="AJ19">
         <v>0</v>
       </c>
+      <c r="AK19" s="5">
+        <f>SUM(B19:AJ19)</f>
+        <v>106</v>
+      </c>
     </row>
-    <row r="20" spans="1:253" ht="13.5">
-      <c r="A20" s="3">
+    <row r="20" ht="13.5">
+      <c r="A20" s="4">
         <v>43926</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="6">
         <v>4</v>
       </c>
       <c r="D20">
@@ -3178,7 +3207,7 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="6">
         <v>103</v>
       </c>
       <c r="I20">
@@ -3262,12 +3291,16 @@
       <c r="AI20">
         <v>0</v>
       </c>
-      <c r="AJ20" s="4">
+      <c r="AJ20" s="6">
         <v>-3</v>
       </c>
+      <c r="AK20" s="5">
+        <f>SUM(B20:AJ20)</f>
+        <v>181</v>
+      </c>
     </row>
-    <row r="21" spans="1:253">
-      <c r="A21" s="3">
+    <row r="21">
+      <c r="A21" s="4">
         <v>43927</v>
       </c>
       <c r="B21">
@@ -3288,7 +3321,7 @@
       <c r="G21">
         <v>6</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="6">
         <v>103</v>
       </c>
       <c r="I21">
@@ -3303,7 +3336,7 @@
       <c r="L21">
         <v>1</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="6">
         <v>0</v>
       </c>
       <c r="N21">
@@ -3339,10 +3372,10 @@
       <c r="X21">
         <v>1</v>
       </c>
-      <c r="Y21" s="4">
+      <c r="Y21" s="6">
         <v>29</v>
       </c>
-      <c r="Z21" s="4">
+      <c r="Z21" s="6">
         <v>1</v>
       </c>
       <c r="AA21">
@@ -3375,9 +3408,13 @@
       <c r="AJ21">
         <v>0</v>
       </c>
+      <c r="AK21" s="5">
+        <f>SUM(B21:AJ21)</f>
+        <v>218</v>
+      </c>
     </row>
-    <row r="22" spans="1:253">
-      <c r="A22" s="3">
+    <row r="22">
+      <c r="A22" s="4">
         <v>43928</v>
       </c>
       <c r="B22">
@@ -3485,9 +3522,13 @@
       <c r="AJ22">
         <v>0</v>
       </c>
+      <c r="AK22" s="5">
+        <f>SUM(B22:AJ22)</f>
+        <v>247</v>
+      </c>
     </row>
-    <row r="23" spans="1:253">
-      <c r="A23" s="3">
+    <row r="23">
+      <c r="A23" s="4">
         <v>43929</v>
       </c>
       <c r="B23">
@@ -3556,10 +3597,10 @@
       <c r="W23">
         <v>33</v>
       </c>
-      <c r="X23" s="4">
+      <c r="X23" s="6">
         <v>3</v>
       </c>
-      <c r="Y23" s="4">
+      <c r="Y23" s="6">
         <v>1</v>
       </c>
       <c r="Z23">
@@ -3595,12 +3636,16 @@
       <c r="AJ23">
         <v>0</v>
       </c>
+      <c r="AK23" s="5">
+        <f>SUM(B23:AJ23)</f>
+        <v>218</v>
+      </c>
     </row>
-    <row r="24" spans="1:253" ht="13.5">
-      <c r="A24" s="3">
+    <row r="24" ht="13.5">
+      <c r="A24" s="4">
         <v>43930</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="6">
         <v>-1</v>
       </c>
       <c r="C24">
@@ -3648,7 +3693,7 @@
       <c r="Q24">
         <v>0</v>
       </c>
-      <c r="R24" s="4">
+      <c r="R24" s="6">
         <v>12</v>
       </c>
       <c r="S24">
@@ -3678,7 +3723,7 @@
       <c r="AA24">
         <v>0</v>
       </c>
-      <c r="AB24" s="4">
+      <c r="AB24" s="6">
         <v>1</v>
       </c>
       <c r="AC24">
@@ -3702,12 +3747,16 @@
       <c r="AI24">
         <v>0</v>
       </c>
-      <c r="AJ24" s="4">
-        <v>1</v>
+      <c r="AJ24" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="5">
+        <f>SUM(B24:AJ24)</f>
+        <v>337</v>
       </c>
     </row>
-    <row r="25" spans="1:253" ht="13.5">
-      <c r="A25" s="3">
+    <row r="25" ht="13.5">
+      <c r="A25" s="4">
         <v>43931</v>
       </c>
       <c r="B25">
@@ -3728,13 +3777,13 @@
       <c r="G25">
         <v>0</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="6">
         <v>46</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="6">
         <v>13</v>
       </c>
       <c r="K25">
@@ -3815,9 +3864,13 @@
       <c r="AJ25">
         <v>0</v>
       </c>
+      <c r="AK25" s="5">
+        <f>SUM(B25:AJ25)</f>
+        <v>219</v>
+      </c>
     </row>
-    <row r="26" spans="1:253" ht="13.5">
-      <c r="A26" s="3">
+    <row r="26" ht="13.5">
+      <c r="A26" s="4">
         <v>43932</v>
       </c>
       <c r="B26">
@@ -3925,9 +3978,13 @@
       <c r="AJ26">
         <v>0</v>
       </c>
+      <c r="AK26" s="5">
+        <f>SUM(B26:AJ26)</f>
+        <v>330</v>
+      </c>
     </row>
-    <row r="27" spans="1:253" ht="13.5">
-      <c r="A27" s="6">
+    <row r="27" ht="13.5">
+      <c r="A27" s="8">
         <v>43933</v>
       </c>
       <c r="B27">
@@ -3948,13 +4005,13 @@
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="6">
         <v>78</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="6">
         <v>59</v>
       </c>
       <c r="K27">
@@ -3984,7 +4041,7 @@
       <c r="S27">
         <v>10</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T27" s="6">
         <v>-3</v>
       </c>
       <c r="U27">
@@ -3999,7 +4056,7 @@
       <c r="X27">
         <v>0</v>
       </c>
-      <c r="Y27" s="4">
+      <c r="Y27" s="6">
         <v>45</v>
       </c>
       <c r="Z27">
@@ -4017,7 +4074,7 @@
       <c r="AD27">
         <v>8</v>
       </c>
-      <c r="AE27" s="4">
+      <c r="AE27" s="6">
         <v>0</v>
       </c>
       <c r="AF27">
@@ -4035,9 +4092,13 @@
       <c r="AJ27">
         <v>-9</v>
       </c>
+      <c r="AK27" s="5">
+        <f>SUM(B27:AJ27)</f>
+        <v>399</v>
+      </c>
     </row>
-    <row r="28" spans="1:253" ht="13.5">
-      <c r="A28" s="6">
+    <row r="28" ht="13.5">
+      <c r="A28" s="8">
         <v>43934</v>
       </c>
       <c r="B28">
@@ -4046,10 +4107,10 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="6">
         <v>-5</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="7">
         <v>0</v>
       </c>
       <c r="F28">
@@ -4058,13 +4119,13 @@
       <c r="G28">
         <v>16</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="6">
         <v>179</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="6">
         <v>50</v>
       </c>
       <c r="K28">
@@ -4109,7 +4170,7 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28" s="4">
+      <c r="Y28" s="6">
         <v>-1</v>
       </c>
       <c r="Z28">
@@ -4142,12 +4203,16 @@
       <c r="AI28">
         <v>0</v>
       </c>
-      <c r="AJ28" s="4">
-        <v>1</v>
+      <c r="AJ28" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="5">
+        <f>SUM(B28:AJ28)</f>
+        <v>316</v>
       </c>
     </row>
-    <row r="29" spans="1:253" ht="13.5">
-      <c r="A29" s="6">
+    <row r="29" ht="13.5">
+      <c r="A29" s="8">
         <v>43935</v>
       </c>
       <c r="B29">
@@ -4156,7 +4221,7 @@
       <c r="C29">
         <v>6</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="6">
         <v>5</v>
       </c>
       <c r="E29">
@@ -4165,7 +4230,7 @@
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="6">
         <v>4</v>
       </c>
       <c r="H29">
@@ -4177,7 +4242,7 @@
       <c r="J29">
         <v>0</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="6">
         <v>76</v>
       </c>
       <c r="L29">
@@ -4225,7 +4290,7 @@
       <c r="Z29">
         <v>0</v>
       </c>
-      <c r="AA29" s="4">
+      <c r="AA29" s="6">
         <v>-1</v>
       </c>
       <c r="AB29">
@@ -4255,9 +4320,13 @@
       <c r="AJ29">
         <v>0</v>
       </c>
+      <c r="AK29" s="5">
+        <f>SUM(B29:AJ29)</f>
+        <v>282</v>
+      </c>
     </row>
-    <row r="30" spans="1:253" ht="13.5">
-      <c r="A30" s="6">
+    <row r="30" ht="13.5">
+      <c r="A30" s="8">
         <v>43936</v>
       </c>
       <c r="B30">
@@ -4365,9 +4434,13 @@
       <c r="AJ30">
         <v>0</v>
       </c>
+      <c r="AK30" s="5">
+        <f>SUM(B30:AJ30)</f>
+        <v>297</v>
+      </c>
     </row>
-    <row r="31" spans="1:253" ht="13.5">
-      <c r="A31" s="6">
+    <row r="31" ht="13.5">
+      <c r="A31" s="8">
         <v>43937</v>
       </c>
       <c r="B31">
@@ -4376,7 +4449,7 @@
       <c r="C31">
         <v>15</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="6">
         <v>19</v>
       </c>
       <c r="E31">
@@ -4385,19 +4458,19 @@
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="G31" s="4">
-        <v>1</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="G31" s="6">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6">
         <v>187</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="6">
         <v>15</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="6">
         <v>7</v>
       </c>
       <c r="L31">
@@ -4418,7 +4491,7 @@
       <c r="Q31">
         <v>8</v>
       </c>
-      <c r="R31" s="4">
+      <c r="R31" s="6">
         <v>7</v>
       </c>
       <c r="S31">
@@ -4436,19 +4509,19 @@
       <c r="W31">
         <v>1</v>
       </c>
-      <c r="X31" s="4">
+      <c r="X31" s="6">
         <v>3</v>
       </c>
-      <c r="Y31" s="4">
+      <c r="Y31" s="6">
         <v>28</v>
       </c>
       <c r="Z31">
         <v>0</v>
       </c>
-      <c r="AA31" s="4">
+      <c r="AA31" s="6">
         <v>6</v>
       </c>
-      <c r="AB31" s="4">
+      <c r="AB31" s="6">
         <v>5</v>
       </c>
       <c r="AC31">
@@ -4472,12 +4545,16 @@
       <c r="AI31">
         <v>3</v>
       </c>
-      <c r="AJ31" s="4">
+      <c r="AJ31" s="6">
         <v>-1</v>
       </c>
+      <c r="AK31" s="5">
+        <f>SUM(B31:AJ31)</f>
+        <v>380</v>
+      </c>
     </row>
-    <row r="32" spans="1:253" ht="13.5">
-      <c r="A32" s="6">
+    <row r="32" ht="13.5">
+      <c r="A32" s="8">
         <v>43938</v>
       </c>
       <c r="B32">
@@ -4585,9 +4662,13 @@
       <c r="AJ32">
         <v>0</v>
       </c>
+      <c r="AK32" s="5">
+        <f>SUM(B32:AJ32)</f>
+        <v>407</v>
+      </c>
     </row>
-    <row r="33" spans="1:253" ht="13.5">
-      <c r="A33" s="6">
+    <row r="33" ht="13.5">
+      <c r="A33" s="8">
         <v>43939</v>
       </c>
       <c r="B33">
@@ -4695,9 +4776,13 @@
       <c r="AJ33">
         <v>0</v>
       </c>
+      <c r="AK33" s="5">
+        <f>SUM(B33:AJ33)</f>
+        <v>325</v>
+      </c>
     </row>
-    <row r="34" spans="1:253" ht="13.5">
-      <c r="A34" s="6">
+    <row r="34" ht="13.5">
+      <c r="A34" s="8">
         <v>43940</v>
       </c>
       <c r="B34">
@@ -4706,7 +4791,7 @@
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="6">
         <v>-9</v>
       </c>
       <c r="E34">
@@ -4718,16 +4803,16 @@
       <c r="G34">
         <v>0</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="6">
         <v>94</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="6">
         <v>81</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="6">
         <v>19</v>
       </c>
       <c r="L34">
@@ -4802,12 +4887,16 @@
       <c r="AI34">
         <v>0</v>
       </c>
-      <c r="AJ34" s="4">
-        <v>1</v>
+      <c r="AJ34" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK34" s="5">
+        <f>SUM(B34:AJ34)</f>
+        <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:253" ht="13.5">
-      <c r="A35" s="6">
+    <row r="35" ht="13.5">
+      <c r="A35" s="8">
         <v>43941</v>
       </c>
       <c r="B35">
@@ -4915,9 +5004,13 @@
       <c r="AJ35">
         <v>0</v>
       </c>
+      <c r="AK35" s="5">
+        <f>SUM(B35:AJ35)</f>
+        <v>185</v>
+      </c>
     </row>
-    <row r="36" spans="1:253" ht="13.5">
-      <c r="A36" s="6">
+    <row r="36" ht="13.5">
+      <c r="A36" s="8">
         <v>43942</v>
       </c>
       <c r="B36">
@@ -4926,8 +5019,8 @@
       <c r="C36">
         <v>10</v>
       </c>
-      <c r="D36">
-        <v>0</v>
+      <c r="D36" s="9">
+        <v>-4</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -4938,8 +5031,8 @@
       <c r="G36">
         <v>3</v>
       </c>
-      <c r="H36">
-        <v>163</v>
+      <c r="H36" s="9">
+        <v>167</v>
       </c>
       <c r="I36">
         <v>5</v>
@@ -5025,9 +5118,13 @@
       <c r="AJ36">
         <v>0</v>
       </c>
+      <c r="AK36" s="5">
+        <f>SUM(B36:AJ36)</f>
+        <v>375</v>
+      </c>
     </row>
-    <row r="37" spans="1:253" ht="13.5">
-      <c r="A37" s="6">
+    <row r="37" ht="13.5">
+      <c r="A37" s="8">
         <v>43943</v>
       </c>
       <c r="B37">
@@ -5048,7 +5145,7 @@
       <c r="G37">
         <v>3</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="6">
         <v>120</v>
       </c>
       <c r="I37">
@@ -5132,12 +5229,16 @@
       <c r="AI37">
         <v>0</v>
       </c>
-      <c r="AJ37" s="4">
+      <c r="AJ37" s="6">
         <v>-1</v>
       </c>
+      <c r="AK37" s="5">
+        <f>SUM(B37:AJ37)</f>
+        <v>283</v>
+      </c>
     </row>
-    <row r="38" spans="1:253" ht="13.5">
-      <c r="A38" s="6">
+    <row r="38" ht="13.5">
+      <c r="A38" s="8">
         <v>43944</v>
       </c>
       <c r="B38">
@@ -5158,13 +5259,13 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="6">
         <v>130</v>
       </c>
       <c r="I38">
         <v>1</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="6">
         <v>25</v>
       </c>
       <c r="K38">
@@ -5245,9 +5346,13 @@
       <c r="AJ38">
         <v>0</v>
       </c>
+      <c r="AK38" s="5">
+        <f>SUM(B38:AJ38)</f>
+        <v>357</v>
+      </c>
     </row>
-    <row r="39" spans="1:253" ht="13.5">
-      <c r="A39" s="6">
+    <row r="39" ht="13.5">
+      <c r="A39" s="8">
         <v>43945</v>
       </c>
       <c r="B39">
@@ -5355,9 +5460,13 @@
       <c r="AJ39">
         <v>0</v>
       </c>
+      <c r="AK39" s="5">
+        <f>SUM(B39:AJ39)</f>
+        <v>436</v>
+      </c>
     </row>
-    <row r="40" spans="1:253" ht="13.5">
-      <c r="A40" s="6">
+    <row r="40" ht="13.5">
+      <c r="A40" s="8">
         <v>43946</v>
       </c>
       <c r="B40">
@@ -5376,7 +5485,7 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="H40">
         <v>85</v>
@@ -5439,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="AB40">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="AC40">
         <v>0</v>
@@ -5465,9 +5574,13 @@
       <c r="AJ40">
         <v>0</v>
       </c>
+      <c r="AK40" s="5">
+        <f>SUM(B40:AJ40)</f>
+        <v>396</v>
+      </c>
     </row>
-    <row r="41" spans="1:253" ht="13.5">
-      <c r="A41" s="6">
+    <row r="41" ht="13.5">
+      <c r="A41" s="8">
         <v>43947</v>
       </c>
       <c r="B41">
@@ -5488,7 +5601,7 @@
       <c r="G41">
         <v>3</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="6">
         <v>115</v>
       </c>
       <c r="I41">
@@ -5569,15 +5682,19 @@
       <c r="AH41">
         <v>0</v>
       </c>
-      <c r="AI41" s="4">
+      <c r="AI41" s="6">
         <v>0</v>
       </c>
       <c r="AJ41">
         <v>0</v>
       </c>
+      <c r="AK41" s="5">
+        <f>SUM(B41:AJ41)</f>
+        <v>275</v>
+      </c>
     </row>
-    <row r="42" spans="1:253" ht="13.5">
-      <c r="A42" s="6">
+    <row r="42" ht="13.5">
+      <c r="A42" s="8">
         <v>43948</v>
       </c>
       <c r="B42">
@@ -5604,7 +5721,7 @@
       <c r="I42">
         <v>0</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="6">
         <v>38</v>
       </c>
       <c r="K42">
@@ -5685,9 +5802,13 @@
       <c r="AJ42">
         <v>1</v>
       </c>
+      <c r="AK42" s="5">
+        <f>SUM(B42:AJ42)</f>
+        <v>214</v>
+      </c>
     </row>
-    <row r="43" spans="1:253" ht="13.5">
-      <c r="A43" s="6">
+    <row r="43" ht="13.5">
+      <c r="A43" s="8">
         <v>43949</v>
       </c>
       <c r="B43">
@@ -5795,9 +5916,13 @@
       <c r="AJ43">
         <v>0</v>
       </c>
+      <c r="AK43" s="5">
+        <f>SUM(B43:AJ43)</f>
+        <v>415</v>
+      </c>
     </row>
-    <row r="44" spans="1:253" ht="13.5">
-      <c r="A44" s="6">
+    <row r="44" ht="13.5">
+      <c r="A44" s="8">
         <v>43950</v>
       </c>
       <c r="B44">
@@ -5818,7 +5943,7 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="6">
         <v>91</v>
       </c>
       <c r="I44">
@@ -5902,12 +6027,16 @@
       <c r="AI44">
         <v>0</v>
       </c>
-      <c r="AJ44" s="4">
+      <c r="AJ44" s="6">
         <v>-1</v>
       </c>
+      <c r="AK44" s="5">
+        <f>SUM(B44:AJ44)</f>
+        <v>260</v>
+      </c>
     </row>
-    <row r="45" spans="1:253" ht="13.5">
-      <c r="A45" s="6">
+    <row r="45" ht="13.5">
+      <c r="A45" s="8">
         <v>43951</v>
       </c>
       <c r="B45">
@@ -6015,9 +6144,13 @@
       <c r="AJ45">
         <v>0</v>
       </c>
+      <c r="AK45" s="5">
+        <f>SUM(B45:AJ45)</f>
+        <v>347</v>
+      </c>
     </row>
-    <row r="46" spans="1:253" ht="13.5">
-      <c r="A46" s="6">
+    <row r="46" ht="13.5">
+      <c r="A46" s="8">
         <v>43952</v>
       </c>
       <c r="B46">
@@ -6047,7 +6180,7 @@
       <c r="J46">
         <v>0</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="6">
         <v>24</v>
       </c>
       <c r="L46">
@@ -6122,12 +6255,16 @@
       <c r="AI46">
         <v>0</v>
       </c>
-      <c r="AJ46" s="4">
+      <c r="AJ46" s="6">
         <v>-2</v>
       </c>
+      <c r="AK46" s="5">
+        <f>SUM(B46:AJ46)</f>
+        <v>433</v>
+      </c>
     </row>
-    <row r="47" spans="1:253" ht="13.5">
-      <c r="A47" s="6">
+    <row r="47" ht="13.5">
+      <c r="A47" s="8">
         <v>43953</v>
       </c>
       <c r="B47">
@@ -6148,13 +6285,13 @@
       <c r="G47">
         <v>10</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="6">
         <v>79</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47" s="6">
         <v>32</v>
       </c>
       <c r="K47">
@@ -6235,9 +6372,13 @@
       <c r="AJ47">
         <v>0</v>
       </c>
+      <c r="AK47" s="5">
+        <f>SUM(B47:AJ47)</f>
+        <v>292</v>
+      </c>
     </row>
-    <row r="48" spans="1:253" ht="13.5">
-      <c r="A48" s="6">
+    <row r="48" ht="13.5">
+      <c r="A48" s="8">
         <v>43954</v>
       </c>
       <c r="B48">
@@ -6264,7 +6405,7 @@
       <c r="I48">
         <v>6</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48" s="6">
         <v>15</v>
       </c>
       <c r="K48">
@@ -6342,12 +6483,16 @@
       <c r="AI48">
         <v>0</v>
       </c>
-      <c r="AJ48" s="4">
+      <c r="AJ48" s="6">
         <v>-2</v>
       </c>
+      <c r="AK48" s="5">
+        <f>SUM(B48:AJ48)</f>
+        <v>349</v>
+      </c>
     </row>
-    <row r="49" spans="1:253" ht="13.5">
-      <c r="A49" s="6">
+    <row r="49" ht="13.5">
+      <c r="A49" s="8">
         <v>43955</v>
       </c>
       <c r="B49">
@@ -6455,9 +6600,13 @@
       <c r="AJ49">
         <v>0</v>
       </c>
+      <c r="AK49" s="5">
+        <f>SUM(B49:AJ49)</f>
+        <v>395</v>
+      </c>
     </row>
-    <row r="50" spans="1:253" ht="13.5">
-      <c r="A50" s="6">
+    <row r="50" ht="13.5">
+      <c r="A50" s="8">
         <v>43956</v>
       </c>
       <c r="B50">
@@ -6565,9 +6714,13 @@
       <c r="AJ50">
         <v>0</v>
       </c>
+      <c r="AK50" s="5">
+        <f>SUM(B50:AJ50)</f>
+        <v>484</v>
+      </c>
     </row>
-    <row r="51" spans="1:253" ht="13.5">
-      <c r="A51" s="6">
+    <row r="51" ht="13.5">
+      <c r="A51" s="8">
         <v>43957</v>
       </c>
       <c r="B51">
@@ -6675,9 +6828,13 @@
       <c r="AJ51">
         <v>0</v>
       </c>
+      <c r="AK51" s="5">
+        <f>SUM(B51:AJ51)</f>
+        <v>367</v>
+      </c>
     </row>
-    <row r="52" spans="1:253" ht="13.5">
-      <c r="A52" s="6">
+    <row r="52" ht="13.5">
+      <c r="A52" s="8">
         <v>43958</v>
       </c>
       <c r="B52">
@@ -6707,7 +6864,7 @@
       <c r="J52">
         <v>61</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K52" s="6">
         <v>14</v>
       </c>
       <c r="L52">
@@ -6782,12 +6939,16 @@
       <c r="AI52">
         <v>4</v>
       </c>
-      <c r="AJ52" s="4">
+      <c r="AJ52" s="6">
         <v>-1</v>
       </c>
+      <c r="AK52" s="5">
+        <f>SUM(B52:AJ52)</f>
+        <v>338</v>
+      </c>
     </row>
-    <row r="53" spans="1:253" ht="13.5">
-      <c r="A53" s="6">
+    <row r="53" ht="13.5">
+      <c r="A53" s="8">
         <v>43959</v>
       </c>
       <c r="B53">
@@ -6895,9 +7056,13 @@
       <c r="AJ53">
         <v>0</v>
       </c>
+      <c r="AK53" s="5">
+        <f>SUM(B53:AJ53)</f>
+        <v>336</v>
+      </c>
     </row>
-    <row r="54" spans="1:253" ht="13.5">
-      <c r="A54" s="6">
+    <row r="54" ht="13.5">
+      <c r="A54" s="8">
         <v>43960</v>
       </c>
       <c r="B54">
@@ -7005,9 +7170,13 @@
       <c r="AJ54">
         <v>0</v>
       </c>
+      <c r="AK54" s="5">
+        <f>SUM(B54:AJ54)</f>
+        <v>533</v>
+      </c>
     </row>
-    <row r="55" spans="1:253" ht="13.5">
-      <c r="A55" s="6">
+    <row r="55" ht="13.5">
+      <c r="A55" s="8">
         <v>43961</v>
       </c>
       <c r="B55">
@@ -7115,9 +7284,13 @@
       <c r="AJ55">
         <v>0</v>
       </c>
+      <c r="AK55" s="5">
+        <f>SUM(B55:AJ55)</f>
+        <v>387</v>
+      </c>
     </row>
-    <row r="56" spans="1:253" ht="13.5">
-      <c r="A56" s="6">
+    <row r="56" ht="13.5">
+      <c r="A56" s="8">
         <v>43962</v>
       </c>
       <c r="B56">
@@ -7225,9 +7398,13 @@
       <c r="AJ56">
         <v>0</v>
       </c>
+      <c r="AK56" s="5">
+        <f>SUM(B56:AJ56)</f>
+        <v>233</v>
+      </c>
     </row>
-    <row r="57" spans="1:253" ht="13.5">
-      <c r="A57" s="6">
+    <row r="57" ht="13.5">
+      <c r="A57" s="8">
         <v>43963</v>
       </c>
       <c r="B57">
@@ -7335,9 +7512,13 @@
       <c r="AJ57">
         <v>0</v>
       </c>
+      <c r="AK57" s="5">
+        <f>SUM(B57:AJ57)</f>
+        <v>484</v>
+      </c>
     </row>
-    <row r="58" spans="1:253" ht="13.5">
-      <c r="A58" s="6">
+    <row r="58" ht="13.5">
+      <c r="A58" s="8">
         <v>43964</v>
       </c>
       <c r="B58">
@@ -7406,14 +7587,14 @@
       <c r="W58">
         <v>2</v>
       </c>
-      <c r="X58">
-        <v>91</v>
+      <c r="X58" s="9">
+        <v>90</v>
       </c>
       <c r="Y58">
         <v>55</v>
       </c>
-      <c r="Z58">
-        <v>6</v>
+      <c r="Z58" s="9">
+        <v>7</v>
       </c>
       <c r="AA58">
         <v>0</v>
@@ -7445,17 +7626,235 @@
       <c r="AJ58">
         <v>0</v>
       </c>
+      <c r="AK58" s="5">
+        <f>SUM(B58:AJ58)</f>
+        <v>689</v>
+      </c>
     </row>
-    <row r="60" spans="1:253" ht="13.5"/>
-    <row r="62" spans="1:253" ht="13.5"/>
+    <row r="59" ht="12.75">
+      <c r="A59" s="8">
+        <v>43965</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>13</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>4</v>
+      </c>
+      <c r="H59">
+        <v>134</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>9</v>
+      </c>
+      <c r="K59">
+        <v>43</v>
+      </c>
+      <c r="L59">
+        <v>91</v>
+      </c>
+      <c r="N59">
+        <v>8</v>
+      </c>
+      <c r="O59">
+        <v>3</v>
+      </c>
+      <c r="P59">
+        <v>3</v>
+      </c>
+      <c r="S59">
+        <v>6</v>
+      </c>
+      <c r="T59">
+        <v>119</v>
+      </c>
+      <c r="U59">
+        <v>32</v>
+      </c>
+      <c r="V59">
+        <v>1</v>
+      </c>
+      <c r="W59">
+        <v>2</v>
+      </c>
+      <c r="Y59">
+        <v>37</v>
+      </c>
+      <c r="Z59">
+        <v>9</v>
+      </c>
+      <c r="AB59">
+        <v>6</v>
+      </c>
+      <c r="AC59">
+        <v>3</v>
+      </c>
+      <c r="AD59">
+        <v>12</v>
+      </c>
+      <c r="AE59">
+        <v>18</v>
+      </c>
+      <c r="AF59">
+        <v>4</v>
+      </c>
+      <c r="AG59">
+        <v>1</v>
+      </c>
+      <c r="AI59">
+        <v>2</v>
+      </c>
+      <c r="AK59" s="5">
+        <f>SUM(B59:AJ59)</f>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="60" ht="13.5">
+      <c r="A60" s="8">
+        <v>43966</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>29</v>
+      </c>
+      <c r="F60">
+        <v>11</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60">
+        <v>86</v>
+      </c>
+      <c r="I60">
+        <v>3</v>
+      </c>
+      <c r="J60">
+        <v>31</v>
+      </c>
+      <c r="K60">
+        <v>43</v>
+      </c>
+      <c r="L60">
+        <v>58</v>
+      </c>
+      <c r="N60">
+        <v>13</v>
+      </c>
+      <c r="O60">
+        <v>4</v>
+      </c>
+      <c r="P60">
+        <v>69</v>
+      </c>
+      <c r="Q60">
+        <v>3</v>
+      </c>
+      <c r="R60">
+        <v>4</v>
+      </c>
+      <c r="S60">
+        <v>8</v>
+      </c>
+      <c r="T60">
+        <v>17</v>
+      </c>
+      <c r="U60">
+        <v>22</v>
+      </c>
+      <c r="V60">
+        <v>22</v>
+      </c>
+      <c r="X60">
+        <v>17</v>
+      </c>
+      <c r="Y60">
+        <v>31</v>
+      </c>
+      <c r="Z60">
+        <v>1</v>
+      </c>
+      <c r="AB60">
+        <v>1</v>
+      </c>
+      <c r="AC60">
+        <v>4</v>
+      </c>
+      <c r="AF60">
+        <v>3</v>
+      </c>
+      <c r="AI60">
+        <v>1</v>
+      </c>
+      <c r="AK60" s="5">
+        <f>SUM(B60:AJ60)</f>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="61" ht="12.75">
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="T61"/>
+      <c r="U61"/>
+      <c r="V61"/>
+      <c r="W61"/>
+      <c r="X61"/>
+      <c r="Y61"/>
+      <c r="Z61"/>
+      <c r="AA61"/>
+      <c r="AB61"/>
+      <c r="AC61"/>
+      <c r="AD61"/>
+      <c r="AE61"/>
+      <c r="AF61"/>
+      <c r="AG61"/>
+      <c r="AH61"/>
+      <c r="AI61"/>
+      <c r="AJ61"/>
+      <c r="AK61"/>
+    </row>
+    <row r="62" ht="13.5"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="0" fitToWidth="0" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>